<commit_message>
se termina logica crud estudiantes
</commit_message>
<xml_diff>
--- a/APP/data/registro.xlsx
+++ b/APP/data/registro.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,42 +470,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Estudiantes-64648d</t>
+          <t>Estudiantes-748160</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Juan Perez</t>
+          <t>Lujan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>62626</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estudiantes-748160</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lujan</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Gomez</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>73243</t>
         </is>

</xml_diff>

<commit_message>
se termina logica crud materias e incripciones
</commit_message>
<xml_diff>
--- a/APP/data/registro.xlsx
+++ b/APP/data/registro.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19050" windowHeight="1560" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +11,7 @@
     <sheet name="Inscripciones" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -52,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -421,7 +420,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <cols>
+    <col width="13.08984375" customWidth="1" min="1" max="1"/>
+    <col width="11.453125" customWidth="1" min="2" max="2"/>
+    <col width="10.26953125" customWidth="1" min="3" max="3"/>
+    <col width="11.81640625" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -500,13 +505,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <cols>
+    <col width="17.1796875" customWidth="1" min="1" max="1"/>
+    <col width="16.36328125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -516,6 +525,11 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>ING</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Ingenieria de Software</t>
         </is>
       </c>
@@ -528,6 +542,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Implementacion en la Nube</t>
         </is>
       </c>
@@ -539,6 +558,11 @@
         </is>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>Desarrollo BackEnd</t>
         </is>
@@ -555,14 +579,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Inscripciones-bb95bb</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Estudiantes-0e66c5</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Materias-0dd25c</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add - campo para fecha de inscripcion a materia
</commit_message>
<xml_diff>
--- a/APP/data/registro.xlsx
+++ b/APP/data/registro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19050" windowHeight="1560" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19050" windowHeight="1560" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" state="visible" r:id="rId1"/>
@@ -47,8 +47,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +421,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="13.08984375" customWidth="1" min="1" max="1"/>
     <col width="11.453125" customWidth="1" min="2" max="2"/>
@@ -505,13 +506,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="17.1796875" customWidth="1" min="1" max="1"/>
     <col width="16.36328125" customWidth="1" min="3" max="3"/>
@@ -565,6 +566,23 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>Desarrollo BackEnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Materias-75e70e</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LOG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Logica computacional</t>
         </is>
       </c>
     </row>
@@ -579,35 +597,76 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="17.6328125" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="13.81640625" customWidth="1" min="3" max="3"/>
+    <col width="26.1796875" customWidth="1" style="1" min="5" max="5"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Inscripciones-bb95bb</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Inscripciones-c2a095</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Estudiantes-0e66c5</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Materias-0dd25c</t>
         </is>
       </c>
-      <c r="D1" t="n">
-        <v>6</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-09-11 09:58:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Inscripciones-77ee5a</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Estudiantes-0e66c5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Materias-6ea3a0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-09-11 10:01:30</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>